<commit_message>
cores nos graficos de barras
</commit_message>
<xml_diff>
--- a/docs/qtd_aluno.xlsx
+++ b/docs/qtd_aluno.xlsx
@@ -25,49 +25,88 @@
     <t>Quantidade</t>
   </si>
   <si>
+    <t>ABEL PEREIRA LIMA SOARES</t>
+  </si>
+  <si>
+    <t>ALEXSANDRA NOGUEIRA MARTINS SILVA</t>
+  </si>
+  <si>
+    <t>AMANDA ALVES REZENDE</t>
+  </si>
+  <si>
+    <t>AMANY HATAE CAMPOVILLE</t>
+  </si>
+  <si>
+    <t>ANA BEATRIZ SILVA BRANDÃO DE SOUZA</t>
+  </si>
+  <si>
+    <t>BÁRBARA ARTUZO SIMABUCO</t>
+  </si>
+  <si>
+    <t>CARLOS EDUARDO DOS SANTOS NASCIMENTO</t>
+  </si>
+  <si>
+    <t>DANIELLE DOS SANTOS BARRETO</t>
+  </si>
+  <si>
+    <t>EDER DE ARRUDA INSAURALDE</t>
+  </si>
+  <si>
+    <t>FERNANDO RIBEIRO DOS SANTOS</t>
+  </si>
+  <si>
     <t>GABRIEL HALLEY FARIA JARD</t>
   </si>
   <si>
+    <t>HENRIQUE RANIERI COVALI PONTES</t>
+  </si>
+  <si>
+    <t>HEVELEN KAILA BARBOSA DE QUEIROZ</t>
+  </si>
+  <si>
+    <t>HIGOR LOPES BERNAL</t>
+  </si>
+  <si>
+    <t>IGOR LIBÓRIO FREITAS</t>
+  </si>
+  <si>
+    <t>ISABELLE ERROBIDARTE DE MATOS</t>
+  </si>
+  <si>
+    <t>LEANDRO NOGUEIRA BOMFIM</t>
+  </si>
+  <si>
+    <t>LEONARDO OLIVEIRA SUCH</t>
+  </si>
+  <si>
+    <t>LETHICIA FARIAS MARCINO</t>
+  </si>
+  <si>
+    <t>LINDEMBERG BARBOSA JUNIOR</t>
+  </si>
+  <si>
     <t>LUANA LARISSA DE CARVALHO FERREIRA</t>
   </si>
   <si>
-    <t>EDER DE ARRUDA INSAURALDE</t>
+    <t>MARCOS TALVANI PEREIRA DE SOUZA</t>
   </si>
   <si>
     <t>MARIA BEATRIZ KIOMIDO MENDONÇA</t>
   </si>
   <si>
-    <t>HEVELEN KAILA BARBOSA DE QUEIROZ</t>
-  </si>
-  <si>
-    <t>IGOR LIBÓRIO FREITAS</t>
-  </si>
-  <si>
-    <t>ABEL PEREIRA LIMA SOARES</t>
-  </si>
-  <si>
-    <t>MARCOS TALVANI PEREIRA DE SOUZA</t>
-  </si>
-  <si>
-    <t>ALEXSANDRA NOGUEIRA MARTINS SILVA</t>
-  </si>
-  <si>
     <t>MAURICIO HIROYUKI KUBO</t>
   </si>
   <si>
-    <t>LINDEMBERG BARBOSA JUNIOR</t>
-  </si>
-  <si>
-    <t>AMANY HATAE CAMPOVILLE</t>
-  </si>
-  <si>
-    <t>FERNANDO RIBEIRO DOS SANTOS</t>
-  </si>
-  <si>
-    <t>ANA BEATRIZ SILVA BRANDÃO DE SOUZA</t>
-  </si>
-  <si>
-    <t>BÁRBARA ARTUZO SIMABUCO</t>
+    <t>RAYANNE ESTER BARBOSA DA SILVA</t>
+  </si>
+  <si>
+    <t>RAÍSSA DE ANDRADE ÁGUAS</t>
+  </si>
+  <si>
+    <t>ROBERT ROGGER DE LIMA</t>
+  </si>
+  <si>
+    <t>VICTOR AUGUSTO ALVES BENTO</t>
   </si>
   <si>
     <t>VICTORIA KETHLYN RICARTES DOS SANTOS</t>
@@ -76,97 +115,58 @@
     <t>WELINGTON OLIVEIRA DE SOUZA DOS ANJOS COSTA</t>
   </si>
   <si>
-    <t>DANIELLE DOS SANTOS BARRETO</t>
-  </si>
-  <si>
-    <t>LEONARDO OLIVEIRA SUCH</t>
-  </si>
-  <si>
-    <t>RAÍSSA DE ANDRADE ÁGUAS</t>
-  </si>
-  <si>
-    <t>AMANDA ALVES REZENDE</t>
-  </si>
-  <si>
-    <t>ISABELLE ERROBIDARTE DE MATOS</t>
-  </si>
-  <si>
-    <t>LEANDRO NOGUEIRA BOMFIM</t>
-  </si>
-  <si>
-    <t>VICTOR AUGUSTO ALVES BENTO</t>
-  </si>
-  <si>
-    <t>HENRIQUE RANIERI COVALI PONTES</t>
-  </si>
-  <si>
     <t>WELLYNGTON MATHEUS SOUZA SANTIAGO</t>
   </si>
   <si>
-    <t>ROBERT ROGGER DE LIMA</t>
-  </si>
-  <si>
-    <t>RAYANNE ESTER BARBOSA DA SILVA</t>
-  </si>
-  <si>
-    <t>HIGOR LOPES BERNAL</t>
-  </si>
-  <si>
-    <t>LETHICIA FARIAS MARCINO</t>
-  </si>
-  <si>
-    <t>CARLOS EDUARDO DOS SANTOS NASCIMENTO</t>
+    <t>CPCS</t>
+  </si>
+  <si>
+    <t>FAMED</t>
+  </si>
+  <si>
+    <t>CPTL</t>
+  </si>
+  <si>
+    <t>FAALC</t>
+  </si>
+  <si>
+    <t>INISA</t>
+  </si>
+  <si>
+    <t>FAED</t>
+  </si>
+  <si>
+    <t>CPAQ</t>
   </si>
   <si>
     <t>CPAN</t>
   </si>
   <si>
-    <t>CPAQ</t>
+    <t>INBIO</t>
   </si>
   <si>
     <t>CPAR</t>
   </si>
   <si>
-    <t>CPCS</t>
+    <t>FAMEZ</t>
+  </si>
+  <si>
+    <t>FAENG</t>
   </si>
   <si>
     <t>CPNV</t>
   </si>
   <si>
-    <t>CPTL</t>
-  </si>
-  <si>
-    <t>FAALC</t>
+    <t>INFI</t>
+  </si>
+  <si>
+    <t>FAODO</t>
   </si>
   <si>
     <t>FACFAN</t>
   </si>
   <si>
     <t>FADIR</t>
-  </si>
-  <si>
-    <t>FAED</t>
-  </si>
-  <si>
-    <t>FAENG</t>
-  </si>
-  <si>
-    <t>FAMED</t>
-  </si>
-  <si>
-    <t>FAMEZ</t>
-  </si>
-  <si>
-    <t>FAODO</t>
-  </si>
-  <si>
-    <t>INBIO</t>
-  </si>
-  <si>
-    <t>INFI</t>
-  </si>
-  <si>
-    <t>INISA</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -590,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -612,7 +612,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -623,7 +623,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -634,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -645,7 +645,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -656,7 +656,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -667,7 +667,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -678,7 +678,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -689,7 +689,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -700,7 +700,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -711,7 +711,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -722,7 +722,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -733,7 +733,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -744,7 +744,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -755,7 +755,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -766,7 +766,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -777,7 +777,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -788,7 +788,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -799,7 +799,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -810,7 +810,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -821,7 +821,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -832,7 +832,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -843,7 +843,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -854,7 +854,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -876,7 +876,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C32">
         <v>2</v>

</xml_diff>